<commit_message>
minor update to spreadsheet
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-wildfly-overlay.xlsx
+++ b/cms-ars-3.1-moderate-wildfly-overlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-wildfly-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{709E1000-A9F9-FE4B-99BC-1D4CB3E3E016}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BB4D7C42-2A07-B146-B9F7-CCBA5BAF38D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67200" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-jboss-wild" sheetId="1" r:id="rId1"/>
@@ -7551,48 +7551,6 @@
       <t>-approved SSL certificates.
 2. Configure the SSL certificate using your certificate values.
 3. Set the SSL protocol to TLS V1.1 or V1.2.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Some networking protocols may not meet organizational security requirements
-to protect data and components.
-    Application servers natively host a number of various features, such as
-management interfaces, httpd servers and message queues. These features all run
-on TCPIP ports. This creates the potential that the vendor may choose to
-utilize port numbers or network services that have been deemed unusable by the
-organization. The application server must have the capability to both
-reconfigure and disable the assigned ports without adversely impacting
-application server operation capabilities. For a list of approved ports and
-protocols, reference the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>DoD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ports and protocols website at
-https://powhatan.iiie.disa.mil/ports/cal.html.</t>
     </r>
   </si>
   <si>
@@ -8217,12 +8175,58 @@
   CA-approved certificates.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Some networking protocols may not meet organizational security requirements
+to protect data and components.
+    Application servers natively host a number of various features, such as
+management interfaces, httpd servers and message queues. These features all run
+on TCPIP ports. This creates the potential that the vendor may choose to
+utilize port numbers or network services that have been deemed unusable by the
+organization. The application server must have the capability to both
+reconfigure and disable the assigned ports without adversely impacting
+application server operation capabilities. </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">For a list of approved ports and
+protocols, reference the </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>DoD</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ports and protocols website at
+https://powhatan.iiie.disa.mil/ports/cal.html.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8367,6 +8371,14 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -9092,7 +9104,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.6640625" defaultRowHeight="16"/>
@@ -10503,14 +10515,14 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="409.6">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="5" t="s">
         <v>349</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>346</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>852</v>
+        <v>864</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>347</v>
@@ -10873,7 +10885,7 @@
         <v>431</v>
       </c>
       <c r="S33" s="4" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="409.6">
@@ -11035,7 +11047,7 @@
         <v>470</v>
       </c>
       <c r="S36" s="4" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="409.6">
@@ -11556,7 +11568,7 @@
         <v>589</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>590</v>
@@ -11626,10 +11638,10 @@
         <v>604</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>856</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>857</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>602</v>
@@ -11659,10 +11671,10 @@
         <v>608</v>
       </c>
       <c r="N48" s="4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="P48" s="1" t="s">
         <v>609</v>
@@ -11785,7 +11797,7 @@
         <v>637</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>634</v>
@@ -11833,7 +11845,7 @@
         <v>646</v>
       </c>
       <c r="S51" s="4" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="409.6">
@@ -12424,10 +12436,10 @@
         <v>779</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>861</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>862</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>777</v>
@@ -12457,10 +12469,10 @@
         <v>783</v>
       </c>
       <c r="N63" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="O63" s="4" t="s">
         <v>863</v>
-      </c>
-      <c r="O63" s="4" t="s">
-        <v>864</v>
       </c>
       <c r="P63" s="1" t="s">
         <v>784</v>

</xml_diff>